<commit_message>
Validating and refreshing performance measure objects
</commit_message>
<xml_diff>
--- a/Objects/PerfMeasures_1a.xlsx
+++ b/Objects/PerfMeasures_1a.xlsx
@@ -509,7 +509,7 @@
         <v>83.05</v>
       </c>
       <c r="M2">
-        <v>4.2</v>
+        <v>4.3</v>
       </c>
       <c r="N2">
         <v>68.7</v>
@@ -579,7 +579,7 @@
         <v>78.77</v>
       </c>
       <c r="M3">
-        <v>3.6</v>
+        <v>3.8</v>
       </c>
       <c r="N3">
         <v>61.4</v>
@@ -649,7 +649,7 @@
         <v>75.67</v>
       </c>
       <c r="M4">
-        <v>3.4</v>
+        <v>3.6</v>
       </c>
       <c r="N4">
         <v>55.8</v>
@@ -719,7 +719,7 @@
         <v>74.09999999999999</v>
       </c>
       <c r="M5">
-        <v>3.3</v>
+        <v>3.4</v>
       </c>
       <c r="N5">
         <v>53.5</v>
@@ -789,7 +789,7 @@
         <v>71.67</v>
       </c>
       <c r="M6">
-        <v>2.7</v>
+        <v>2.8</v>
       </c>
       <c r="N6">
         <v>49.1</v>
@@ -847,7 +847,7 @@
         <v>11.3</v>
       </c>
       <c r="I7">
-        <v>0.1128871063179595</v>
+        <v>0.112906918401084</v>
       </c>
       <c r="J7">
         <v>68.7</v>
@@ -859,7 +859,7 @@
         <v>69.47</v>
       </c>
       <c r="M7">
-        <v>2.4</v>
+        <v>2.5</v>
       </c>
       <c r="N7">
         <v>43.7</v>
@@ -929,7 +929,7 @@
         <v>68.68000000000001</v>
       </c>
       <c r="M8">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="N8">
         <v>43.1</v>

</xml_diff>